<commit_message>
wrapping up pca, getting closer to a final version of diomensionality reduction in demographics
</commit_message>
<xml_diff>
--- a/Files/demographic_pca.xlsx
+++ b/Files/demographic_pca.xlsx
@@ -475,16 +475,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.3551707882428473</v>
+        <v>-0.3551707877185219</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3309289999810216</v>
+        <v>0.3309290034432869</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1357932221772313</v>
+        <v>0.1357936041306777</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06561942913576983</v>
+        <v>0.06559983336852679</v>
       </c>
     </row>
     <row r="3">
@@ -494,16 +494,16 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.8363621325053934</v>
+        <v>-0.8363621319867472</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3374123880085946</v>
+        <v>0.3374123827944999</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.08660979487546677</v>
+        <v>-0.08660961873298782</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1458631499225425</v>
+        <v>-0.1458699341423294</v>
       </c>
     </row>
     <row r="4">
@@ -513,16 +513,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3631528497342701</v>
+        <v>0.3631528500888902</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2068930504673</v>
+        <v>-0.2068930501714083</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1286104382052951</v>
+        <v>0.1286105224588112</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.3494065239204669</v>
+        <v>-0.3494029857183761</v>
       </c>
     </row>
     <row r="5">
@@ -532,16 +532,16 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.5982532274642074</v>
+        <v>0.5982532276116911</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.3170466351761435</v>
+        <v>-0.3170466347861214</v>
       </c>
       <c r="D5" t="n">
-        <v>0.15261295163299</v>
+        <v>0.1526129889600649</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>-0.4792131765472138</v>
+        <v>-0.4792115317368918</v>
       </c>
     </row>
     <row r="6">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.7236782496668909</v>
+        <v>0.7236782496885217</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3495330829371723</v>
+        <v>-0.3495330837594584</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1232410231130509</v>
+        <v>0.1232410614585505</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.4228884585180965</v>
+        <v>-0.4228928228177335</v>
       </c>
     </row>
     <row r="7">
@@ -570,16 +570,16 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.8681419013541347</v>
+        <v>0.8681419014628066</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.3625633477433023</v>
+        <v>-0.3625633479101736</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1529629520784823</v>
+        <v>0.1529629989619011</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.09255928649498599</v>
+        <v>-0.09256078494914327</v>
       </c>
     </row>
     <row r="8">
@@ -589,16 +589,16 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0.8412784600560789</v>
+        <v>0.8412784600578528</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.4054813247967586</v>
+        <v>-0.4054813253990132</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1732715047099029</v>
+        <v>0.1732714936826199</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1593913904157285</v>
+        <v>0.1593920402211718</v>
       </c>
     </row>
     <row r="9">
@@ -608,16 +608,16 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>-0.8536099417153165</v>
+        <v>-0.8536099418651647</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3557052474632357</v>
+        <v>0.3557052491784235</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1466514364566719</v>
+        <v>-0.1466514850078401</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.3036632762241487</v>
+        <v>-0.3036612934473726</v>
       </c>
     </row>
     <row r="10">
@@ -627,16 +627,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1279971912495848</v>
+        <v>0.1279971896723688</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.3287583409601018</v>
+        <v>-0.3287583205153982</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.08109128759239159</v>
+        <v>-0.08109173442830026</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.03078944751430011</v>
+        <v>-0.03077324603900185</v>
       </c>
     </row>
     <row r="11">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1016489232776568</v>
+        <v>0.1016489218453303</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.3001663289926422</v>
+        <v>-0.3001663144061094</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1735052022308309</v>
+        <v>-0.1735056745115924</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01384212870037451</v>
+        <v>0.01385949497697186</v>
       </c>
     </row>
     <row r="12">
@@ -665,16 +665,16 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>-0.6645729380667142</v>
+        <v>-0.6645729380611824</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.4003742229631189</v>
+        <v>-0.4003742230803783</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.6056717636212517</v>
+        <v>0.6056717646415741</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02293377398930009</v>
+        <v>0.02293372872521047</v>
       </c>
     </row>
     <row r="13">
@@ -684,16 +684,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3538859613638974</v>
+        <v>0.3538859610292637</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>0.5401543624204128</v>
+        <v>0.5401543599966409</v>
       </c>
       <c r="D13" t="n">
-        <v>0.09532375066480528</v>
+        <v>0.09532350644066918</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.05086623335890122</v>
+        <v>-0.05085403075275857</v>
       </c>
     </row>
     <row r="14">
@@ -703,16 +703,16 @@
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>0.5392787671453594</v>
+        <v>0.5392787672776458</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.1344584541699468</v>
+        <v>-0.1344584550318532</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>-0.7725490722604121</v>
+        <v>-0.7725490171161434</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.09557346606063363</v>
+        <v>-0.09557580245743912</v>
       </c>
     </row>
     <row r="15">
@@ -722,16 +722,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09051742093744246</v>
+        <v>0.09051741910533918</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>0.4567288970070758</v>
+        <v>0.4567289014671995</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0918131115176051</v>
+        <v>-0.09181403596497972</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.1166786066078005</v>
+        <v>-0.1166369662647889</v>
       </c>
     </row>
     <row r="16">
@@ -741,16 +741,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.05038145509183714</v>
+        <v>0.0503814551674826</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01109749129581277</v>
+        <v>0.01109749164325089</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02414172268031619</v>
+        <v>0.02414177737155424</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.01052683740496669</v>
+        <v>-0.01052979089643791</v>
       </c>
     </row>
     <row r="17">
@@ -760,16 +760,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3030622277123918</v>
+        <v>0.3030622290613279</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>0.5150708935026254</v>
+        <v>0.5150708967140337</v>
       </c>
       <c r="D17" t="n">
-        <v>0.04953689899725904</v>
+        <v>0.04953772288004056</v>
       </c>
       <c r="E17" t="n">
-        <v>0.003873788746107655</v>
+        <v>0.00383473922350856</v>
       </c>
     </row>
     <row r="18">
@@ -779,16 +779,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.4383581119049092</v>
+        <v>-0.4383581120574978</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>-0.7949317704778474</v>
+        <v>-0.7949317698723992</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.2773459199299387</v>
+        <v>-0.2773459930551087</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01783617151753953</v>
+        <v>0.01783945222799679</v>
       </c>
     </row>
     <row r="19">
@@ -798,16 +798,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4418549364632182</v>
+        <v>0.4418549363916233</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>0.7458257345034177</v>
+        <v>0.7458257346070263</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3022783681487839</v>
+        <v>0.3022783298630586</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.1517073525065387</v>
+        <v>-0.1517055601469121</v>
       </c>
     </row>
     <row r="20">
@@ -817,16 +817,16 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>-0.561524731802069</v>
+        <v>-0.5615247317024128</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>-0.7266349440803762</v>
+        <v>-0.7266349445766809</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.159503187706822</v>
+        <v>-0.1595031427555744</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.03803287395036212</v>
+        <v>-0.0380348161828063</v>
       </c>
     </row>
     <row r="21">
@@ -836,16 +836,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.0524635809059516</v>
+        <v>-0.05246358148975782</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.2585143905168451</v>
+        <v>-0.2585143873971739</v>
       </c>
       <c r="D21" t="n">
-        <v>0.02404593246511891</v>
+        <v>0.02404567030741708</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.3972521310288524</v>
+        <v>-0.3972405604945621</v>
       </c>
     </row>
     <row r="22">
@@ -855,16 +855,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.02025283272251898</v>
+        <v>-0.02025283344380414</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.3247758607016963</v>
+        <v>-0.324775855075716</v>
       </c>
       <c r="D22" t="n">
-        <v>0.09143422936207829</v>
+        <v>0.09143394919738279</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.4007590445670614</v>
+        <v>-0.4007476183357435</v>
       </c>
     </row>
     <row r="23">
@@ -874,16 +874,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.1036429668003194</v>
+        <v>0.1036429669523971</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.3460332276019049</v>
+        <v>-0.3460332287094098</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2293952426170025</v>
+        <v>0.2293953079952398</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>-0.4734362345364647</v>
+        <v>-0.4734394164381361</v>
       </c>
     </row>
     <row r="24">
@@ -893,16 +893,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.05189572135568425</v>
+        <v>0.05189572145782319</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.2434436014156899</v>
+        <v>-0.2434436026650348</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2065400572181187</v>
+        <v>0.2065400855744932</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.4139263528489528</v>
+        <v>-0.4139271711632105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>